<commit_message>
feat: Introduce SalesModule views for CRM and logistics functionalities, and add numerous reference assets.
</commit_message>
<xml_diff>
--- a/attached_assets/AEROPUERTOS_PRINCIPALES_DEL_MUNDO_1765568483184.xlsx
+++ b/attached_assets/AEROPUERTOS_PRINCIPALES_DEL_MUNDO_1765568483184.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abenincasa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\proyectos\clone_ag__prueba_pytoflutter_importayaia_v2\referencia-ImportaYAia-python\attached_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D3C5BA6-1F09-4816-9E67-540B58041170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D25CA23-044B-4422-BBF8-9AEDA4220E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{896A1D67-A2AC-4C7E-B49E-AE801F69E5CE}"/>
   </bookViews>
@@ -1135,6 +1135,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD623F9F-33D0-4F02-9915-BBAE009BA831}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1527,7 +1530,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1807,6 +1811,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2102,6 +2107,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2330,6 +2336,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2439,5 +2446,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>